<commit_message>
84 airwires left. Did not make the deadline
</commit_message>
<xml_diff>
--- a/PCB_rev_A2/Replicape_BOM_rev_A2.xlsx
+++ b/PCB_rev_A2/Replicape_BOM_rev_A2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
   <si>
     <t>Implemented</t>
   </si>
@@ -245,10 +245,10 @@
     <t>IC REG BUCK SYNC 5V 1A 16-VQFN</t>
   </si>
   <si>
-    <t>LM2596DSADJR4GOSCT-ND</t>
-  </si>
-  <si>
-    <t>IC REG BUCK ADJ 3A D2PAK-5</t>
+    <t>1028-1045-1-ND</t>
+  </si>
+  <si>
+    <t>IC REG BUCK ADJ 2A 10MSOP</t>
   </si>
   <si>
     <t>Resistors</t>
@@ -287,6 +287,12 @@
     <t>RES 0.1 OHM 1/4W 1% 0805 SMD</t>
   </si>
   <si>
+    <t>RMCF0402FT120KCT-ND</t>
+  </si>
+  <si>
+    <t>RES 120K OHM 1/16W 1% 0402</t>
+  </si>
+  <si>
     <t>P5.6KJCT-ND</t>
   </si>
   <si>
@@ -371,6 +377,24 @@
     <t>C12</t>
   </si>
   <si>
+    <t>445-3469-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V Y5V 1206</t>
+  </si>
+  <si>
+    <t>311-1464-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 6.3V 20% X5R 0805</t>
+  </si>
+  <si>
+    <t>445-1257-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 2200PF 50V 10% X7R 0402</t>
+  </si>
+  <si>
     <t>Other</t>
   </si>
   <si>
@@ -416,7 +440,25 @@
     <t>DIODE SCHOTTKY 40V 3A SMA</t>
   </si>
   <si>
-    <t>D1, D2, D3</t>
+    <t>D1, D2, D3, D4, D5, D6, D7</t>
+  </si>
+  <si>
+    <t>445-6517-1-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR POWER 4.7UH 2.0A SMD</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>587-2636-1-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR 33UH 1.7A 20% SMD</t>
+  </si>
+  <si>
+    <t>L2</t>
   </si>
   <si>
     <t>Sum</t>
@@ -643,10 +685,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F28" activeCellId="0" pane="topLeft" sqref="F28"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F58" activeCellId="0" pane="topLeft" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -654,7 +696,13 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3372549019608"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.5882352941176"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.62352941176471"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.47843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.21176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.82352941176471"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.67450980392157"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.4117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.8705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -1468,7 +1516,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>74</v>
@@ -1499,7 +1547,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>76</v>
@@ -1512,22 +1560,22 @@
         <v>1</v>
       </c>
       <c r="F28" s="6" t="n">
-        <v>1.83</v>
+        <v>0.76</v>
       </c>
       <c r="G28" s="7" t="n">
         <f aca="false">F28*E28</f>
-        <v>1.83</v>
+        <v>0.76</v>
       </c>
       <c r="H28" s="6" t="n">
         <f aca="false">500*E28</f>
         <v>500</v>
       </c>
       <c r="I28" s="6" t="n">
-        <v>1.18452</v>
+        <v>0.38192</v>
       </c>
       <c r="J28" s="7" t="n">
         <f aca="false">I28*H28</f>
-        <v>592.26</v>
+        <v>190.96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
@@ -1675,638 +1723,810 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="B35" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="3" t="n">
+      <c r="C35" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F35" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="G34" s="3" t="n">
-        <f aca="false">E34*F34</f>
+      <c r="G35" s="3" t="n">
+        <f aca="false">E35*F35</f>
         <v>0.3</v>
       </c>
-      <c r="H34" s="3" t="n">
+      <c r="H35" s="3" t="n">
         <v>1500</v>
       </c>
-      <c r="I34" s="3" t="n">
+      <c r="I35" s="3" t="n">
         <v>0.0072</v>
       </c>
-      <c r="J34" s="3" t="n">
-        <f aca="false">H34*I34</f>
+      <c r="J35" s="3" t="n">
+        <f aca="false">H35*I35</f>
         <v>10.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
-      <c r="B35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
-      <c r="B36" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="C36" s="14"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="B37" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="3" t="n">
+      <c r="C37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="F37" s="3" t="n">
         <v>0.87</v>
       </c>
-      <c r="G36" s="3" t="n">
-        <f aca="false">E36*F36</f>
+      <c r="G37" s="3" t="n">
+        <f aca="false">E37*F37</f>
         <v>2.61</v>
       </c>
-      <c r="H36" s="3" t="n">
-        <f aca="false">E36*500</f>
-        <v>1500</v>
-      </c>
-      <c r="I36" s="3" t="n">
-        <v>0.3465</v>
-      </c>
-      <c r="J36" s="3" t="n">
-        <f aca="false">H36*I36</f>
-        <v>519.75</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
-      <c r="A37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F37" s="7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G37" s="7" t="n">
-        <f aca="false">E37*F37</f>
-        <v>2.4</v>
-      </c>
-      <c r="H37" s="7" t="n">
+      <c r="H37" s="3" t="n">
         <f aca="false">E37*500</f>
         <v>1500</v>
       </c>
-      <c r="I37" s="6" t="n">
+      <c r="I37" s="3" t="n">
+        <v>0.3465</v>
+      </c>
+      <c r="J37" s="3" t="n">
+        <f aca="false">H37*I37</f>
+        <v>519.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F38" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G38" s="7" t="n">
+        <f aca="false">E38*F38</f>
+        <v>2.4</v>
+      </c>
+      <c r="H38" s="7" t="n">
+        <f aca="false">E38*500</f>
+        <v>1500</v>
+      </c>
+      <c r="I38" s="6" t="n">
         <v>0.4004</v>
       </c>
-      <c r="J37" s="7" t="n">
-        <f aca="false">H37*I37</f>
+      <c r="J38" s="7" t="n">
+        <f aca="false">H38*I38</f>
         <v>600.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
-      <c r="B38" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="9" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
+      <c r="B39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="9" t="n">
+      <c r="E39" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9" t="n">
         <v>1.59</v>
       </c>
-      <c r="G38" s="11" t="n">
-        <f aca="false">E38*F38</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="9" t="n">
-        <f aca="false">E38*500</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="9" t="n">
+      <c r="G39" s="11" t="n">
+        <f aca="false">E39*F39</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="9" t="n">
+        <f aca="false">E39*500</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="9" t="n">
         <v>0.59474</v>
       </c>
-      <c r="J38" s="9" t="n">
-        <f aca="false">H38*I38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
-      <c r="B40" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
+      <c r="J39" s="9" t="n">
+        <f aca="false">H39*I39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
-      <c r="B41" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
+      <c r="B42" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="C42" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F42" s="3" t="n">
         <v>0.15</v>
       </c>
-      <c r="G41" s="3" t="n">
-        <f aca="false">E41*F41</f>
+      <c r="G42" s="3" t="n">
+        <f aca="false">E42*F42</f>
         <v>1.2</v>
       </c>
-      <c r="H41" s="3" t="n">
-        <f aca="false">E41*500</f>
+      <c r="H42" s="3" t="n">
+        <f aca="false">E42*500</f>
         <v>4000</v>
       </c>
-      <c r="I41" s="3" t="n">
+      <c r="I42" s="3" t="n">
         <v>0.02899</v>
       </c>
-      <c r="J41" s="3" t="n">
-        <f aca="false">H41*I41</f>
+      <c r="J42" s="3" t="n">
+        <f aca="false">H42*I42</f>
         <v>115.96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
-      <c r="B42" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="9" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
+      <c r="B43" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="9" t="n">
+      <c r="C43" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="9" t="n">
         <v>0.16</v>
       </c>
-      <c r="G42" s="9" t="n">
-        <f aca="false">E42*F42</f>
-        <v>0</v>
-      </c>
-      <c r="H42" s="9" t="n">
-        <f aca="false">E42*500</f>
-        <v>0</v>
-      </c>
-      <c r="I42" s="9" t="n">
+      <c r="G43" s="9" t="n">
+        <f aca="false">E43*F43</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="9" t="n">
+        <f aca="false">E43*500</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="9" t="n">
         <v>0.0302</v>
       </c>
-      <c r="J42" s="9" t="n">
-        <f aca="false">H42*I42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
-      <c r="A43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="J43" s="9" t="n">
+        <f aca="false">H43*I43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
+      <c r="A44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E43" s="17" t="n">
+      <c r="C44" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="17" t="n">
         <v>21</v>
       </c>
-      <c r="F43" s="3" t="n">
+      <c r="F44" s="3" t="n">
         <v>0.041</v>
-      </c>
-      <c r="G43" s="3" t="n">
-        <f aca="false">E43*F43</f>
-        <v>0.861</v>
-      </c>
-      <c r="H43" s="3" t="n">
-        <f aca="false">E43*500</f>
-        <v>10500</v>
-      </c>
-      <c r="I43" s="3" t="n">
-        <v>0.0102</v>
-      </c>
-      <c r="J43" s="3" t="n">
-        <f aca="false">H43*I43</f>
-        <v>107.1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
-      <c r="B44" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F44" s="3" t="n">
-        <v>0.1</v>
       </c>
       <c r="G44" s="3" t="n">
         <f aca="false">E44*F44</f>
-        <v>0.5</v>
+        <v>0.861</v>
       </c>
       <c r="H44" s="3" t="n">
         <f aca="false">E44*500</f>
-        <v>2500</v>
+        <v>10500</v>
       </c>
       <c r="I44" s="3" t="n">
-        <v>0.00648</v>
+        <v>0.0102</v>
       </c>
       <c r="J44" s="3" t="n">
         <f aca="false">H44*I44</f>
+        <v>107.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
+      <c r="B45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G45" s="3" t="n">
+        <f aca="false">E45*F45</f>
+        <v>0.5</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <f aca="false">E45*500</f>
+        <v>2500</v>
+      </c>
+      <c r="I45" s="3" t="n">
+        <v>0.00648</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <f aca="false">H45*I45</f>
         <v>16.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
-      <c r="B45" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
+      <c r="B46" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E45" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F45" s="5" t="n">
+      <c r="C46" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5" t="n">
         <v>0.81</v>
       </c>
-      <c r="G45" s="3" t="n">
-        <f aca="false">F45*E45</f>
+      <c r="G46" s="3" t="n">
+        <f aca="false">F46*E46</f>
         <v>0.81</v>
       </c>
-      <c r="H45" s="5" t="n">
+      <c r="H46" s="5" t="n">
+        <f aca="false">500*E46</f>
         <v>500</v>
       </c>
-      <c r="I45" s="5" t="n">
+      <c r="I46" s="5" t="n">
         <v>0.33496</v>
       </c>
-      <c r="J45" s="3" t="n">
-        <f aca="false">I45*H45</f>
+      <c r="J46" s="3" t="n">
+        <f aca="false">I46*H46</f>
         <v>167.48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5" t="n">
-        <v>1524</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="3"/>
-    </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
-      <c r="B47" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="3"/>
+      <c r="B47" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" s="6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G47" s="7" t="n">
+        <f aca="false">F47*E47</f>
+        <v>0.5</v>
+      </c>
+      <c r="H47" s="6" t="n">
+        <f aca="false">500*E47</f>
+        <v>1000</v>
+      </c>
+      <c r="I47" s="6" t="n">
+        <v>0.0689</v>
+      </c>
+      <c r="J47" s="7" t="n">
+        <f aca="false">I47*H47</f>
+        <v>68.9</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
-      <c r="B48" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E48" s="3" t="n">
+      <c r="B48" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" s="6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G48" s="7" t="n">
+        <f aca="false">F48*E48</f>
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="6" t="n">
+        <f aca="false">500*E48</f>
+        <v>1000</v>
+      </c>
+      <c r="I48" s="6" t="n">
+        <v>0.06964</v>
+      </c>
+      <c r="J48" s="7" t="n">
+        <f aca="false">I48*H48</f>
+        <v>69.64</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="B49" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G49" s="7" t="n">
+        <f aca="false">F49*E49</f>
+        <v>0.1</v>
+      </c>
+      <c r="H49" s="6" t="n">
+        <f aca="false">500*E49</f>
+        <v>500</v>
+      </c>
+      <c r="I49" s="6" t="n">
+        <v>0.0077</v>
+      </c>
+      <c r="J49" s="7" t="n">
+        <f aca="false">I49*H49</f>
+        <v>3.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51">
+      <c r="B51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
+      <c r="B52" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F52" s="3" t="n">
         <v>0.21</v>
       </c>
-      <c r="G48" s="3" t="n">
-        <f aca="false">E48*F48</f>
+      <c r="G52" s="3" t="n">
+        <f aca="false">E52*F52</f>
         <v>1.47</v>
       </c>
-      <c r="H48" s="3" t="n">
-        <f aca="false">E48*500</f>
+      <c r="H52" s="3" t="n">
+        <f aca="false">E52*500</f>
         <v>3500</v>
       </c>
-      <c r="I48" s="3" t="n">
+      <c r="I52" s="3" t="n">
         <v>0.11178</v>
       </c>
-      <c r="J48" s="3" t="n">
-        <f aca="false">H48*I48</f>
+      <c r="J52" s="3" t="n">
+        <f aca="false">H52*I52</f>
         <v>391.23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49" s="5">
-      <c r="B49" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E49" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" s="3" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53" s="5">
+      <c r="B53" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="G49" s="3" t="n">
-        <f aca="false">E49*F49</f>
+      <c r="G53" s="3" t="n">
+        <f aca="false">E53*F53</f>
         <v>0.6</v>
       </c>
-      <c r="H49" s="3" t="n">
-        <f aca="false">E49*500</f>
+      <c r="H53" s="3" t="n">
+        <f aca="false">E53*500</f>
         <v>500</v>
       </c>
-      <c r="I49" s="3" t="n">
+      <c r="I53" s="3" t="n">
         <v>0.43302</v>
       </c>
-      <c r="J49" s="3" t="n">
-        <f aca="false">H49*I49</f>
+      <c r="J53" s="3" t="n">
+        <f aca="false">H53*I53</f>
         <v>216.51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50" s="5">
-      <c r="A50" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E50" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="n">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54" s="5">
+      <c r="A54" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" s="7" t="n">
         <v>0.83</v>
       </c>
-      <c r="G50" s="7" t="n">
-        <f aca="false">E50*F50</f>
+      <c r="G54" s="7" t="n">
+        <f aca="false">E54*F54</f>
         <v>0.83</v>
       </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="51" s="5">
-      <c r="A51" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E51" s="7" t="n">
+      <c r="H54" s="7" t="n">
+        <f aca="false">E54*500</f>
+        <v>500</v>
+      </c>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55" s="5">
+      <c r="A55" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E55" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F51" s="7" t="n">
+      <c r="F55" s="7" t="n">
         <v>0.56</v>
       </c>
-      <c r="G51" s="7" t="n">
-        <f aca="false">E51*F51</f>
+      <c r="G55" s="7" t="n">
+        <f aca="false">E55*F55</f>
         <v>1.12</v>
       </c>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52" s="5">
-      <c r="A52" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E52" s="7" t="n">
+      <c r="H55" s="7" t="n">
+        <f aca="false">E55*500</f>
+        <v>1000</v>
+      </c>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56" s="5">
+      <c r="A56" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="F52" s="6" t="n">
+      <c r="F56" s="6" t="n">
         <v>0.53</v>
       </c>
-      <c r="G52" s="7" t="n">
-        <f aca="false">E52*F52</f>
+      <c r="G56" s="7" t="n">
+        <f aca="false">E56*F56</f>
         <v>3.18</v>
       </c>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
-      <c r="B53" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1" t="n">
-        <f aca="false">SUM(G3:G52)</f>
-        <v>90.013</v>
-      </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1" t="n">
-        <f aca="false">SUM(J3:J49)/500</f>
-        <v>41.27306</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
-      <c r="B55" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
-      <c r="B56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F56" s="5" t="n">
+      <c r="H56" s="7" t="n">
+        <f aca="false">E56*500</f>
+        <v>3000</v>
+      </c>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57" s="5">
+      <c r="A57" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" s="6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G57" s="7" t="n">
+        <f aca="false">E57*F57</f>
+        <v>0.45</v>
+      </c>
+      <c r="H57" s="7" t="n">
+        <f aca="false">E57*500</f>
+        <v>500</v>
+      </c>
+      <c r="I57" s="6" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="J57" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58" s="5">
+      <c r="A58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" s="6" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7" t="n">
+        <f aca="false">E58*500</f>
+        <v>500</v>
+      </c>
+      <c r="I58" s="6" t="n">
+        <v>0.37126</v>
+      </c>
+      <c r="J58" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="B59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="n">
+        <f aca="false">SUM(G3:G56)</f>
+        <v>90.043</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1" t="n">
+        <f aca="false">SUM(J3:J53)/500</f>
+        <v>40.75524</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="B61" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="B62" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="5" t="n">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="57">
-      <c r="B57" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E57" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F57" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="63">
+      <c r="B63" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="0" t="n">
         <v>69.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="65">
-      <c r="B65" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="B66" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
+      <c r="B71" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
+      <c r="B72" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" s="0" t="n">
         <v>4.04</v>
       </c>
-      <c r="G66" s="0" t="n">
-        <f aca="false">F66*E66</f>
+      <c r="G72" s="0" t="n">
+        <f aca="false">F72*E72</f>
         <v>4.04</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67">
-      <c r="B67" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="E67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
+      <c r="B73" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="G67" s="0" t="n">
-        <f aca="false">F67*E67</f>
+      <c r="G73" s="0" t="n">
+        <f aca="false">F73*E73</f>
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68">
-      <c r="B68" s="5" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
+      <c r="B74" s="5" t="n">
         <v>889740626</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F68" s="0" t="n">
+      <c r="C74" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G68" s="18" t="n">
-        <f aca="false">F68*E68</f>
+      <c r="G74" s="18" t="n">
+        <f aca="false">F74*E74</f>
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69">
-      <c r="B69" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="G69" s="1" t="n">
-        <f aca="false">SUM(G66:G68)</f>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
+      <c r="B75" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="G75" s="1" t="n">
+        <f aca="false">SUM(G72:G74)</f>
         <v>33.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
64 airwires left to route
</commit_message>
<xml_diff>
--- a/PCB_rev_A2/Replicape_BOM_rev_A2.xlsx
+++ b/PCB_rev_A2/Replicape_BOM_rev_A2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="171">
   <si>
     <t>Implemented</t>
   </si>
@@ -459,6 +459,24 @@
   </si>
   <si>
     <t>L2</t>
+  </si>
+  <si>
+    <t>F4266-ND</t>
+  </si>
+  <si>
+    <t>FUSE BLADE 20A/32V MINI FAST-AC</t>
+  </si>
+  <si>
+    <t>F4-1</t>
+  </si>
+  <si>
+    <t>BK-6013-ND</t>
+  </si>
+  <si>
+    <t>FUSE CLIP AUTO 0.110X0.032"BLADE</t>
+  </si>
+  <si>
+    <t>F4</t>
   </si>
   <si>
     <t>Sum</t>
@@ -685,10 +703,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F58" activeCellId="0" pane="topLeft" sqref="F58"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A54" activeCellId="0" pane="topLeft" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -2262,8 +2280,13 @@
         <f aca="false">E54*500</f>
         <v>500</v>
       </c>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
+      <c r="I54" s="6" t="n">
+        <v>0.5421</v>
+      </c>
+      <c r="J54" s="7" t="n">
+        <f aca="false">H54*I54</f>
+        <v>271.05</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55" s="5">
       <c r="A55" s="5" t="n">
@@ -2292,8 +2315,13 @@
         <f aca="false">E55*500</f>
         <v>1000</v>
       </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
+      <c r="I55" s="6" t="n">
+        <v>0.36076</v>
+      </c>
+      <c r="J55" s="7" t="n">
+        <f aca="false">H55*I55</f>
+        <v>360.76</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56" s="5">
       <c r="A56" s="5" t="n">
@@ -2322,8 +2350,13 @@
         <f aca="false">E56*500</f>
         <v>3000</v>
       </c>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
+      <c r="I56" s="6" t="n">
+        <v>0.24812</v>
+      </c>
+      <c r="J56" s="7" t="n">
+        <f aca="false">H56*I56</f>
+        <v>744.36</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57" s="5">
       <c r="A57" s="5" t="n">
@@ -2355,11 +2388,14 @@
       <c r="I57" s="6" t="n">
         <v>0.26</v>
       </c>
-      <c r="J57" s="7"/>
+      <c r="J57" s="7" t="n">
+        <f aca="false">H57*I57</f>
+        <v>130</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58" s="5">
       <c r="A58" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>145</v>
@@ -2376,7 +2412,10 @@
       <c r="F58" s="6" t="n">
         <v>0.57</v>
       </c>
-      <c r="G58" s="7"/>
+      <c r="G58" s="7" t="n">
+        <f aca="false">E58*F58</f>
+        <v>0.57</v>
+      </c>
       <c r="H58" s="7" t="n">
         <f aca="false">E58*500</f>
         <v>500</v>
@@ -2384,149 +2423,216 @@
       <c r="I58" s="6" t="n">
         <v>0.37126</v>
       </c>
-      <c r="J58" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
-      <c r="B59" s="1" t="s">
+      <c r="J58" s="7" t="n">
+        <f aca="false">H58*I58</f>
+        <v>185.63</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59" s="5">
+      <c r="A59" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1" t="n">
-        <f aca="false">SUM(G3:G56)</f>
-        <v>90.043</v>
-      </c>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1" t="n">
+      <c r="C59" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E59" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" s="6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G59" s="7" t="n">
+        <f aca="false">E59*F59</f>
+        <v>0.4</v>
+      </c>
+      <c r="H59" s="7"/>
+      <c r="I59" s="6" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="J59" s="7" t="n">
+        <f aca="false">H59*I59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60" s="5">
+      <c r="A60" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" s="6" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="G60" s="7" t="n">
+        <f aca="false">E60*F60</f>
+        <v>0.47</v>
+      </c>
+      <c r="H60" s="7"/>
+      <c r="I60" s="6" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="J60" s="7" t="n">
+        <f aca="false">H60*I60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="B61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1" t="n">
+        <f aca="false">SUM(G3:G60)</f>
+        <v>91.933</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1" t="n">
         <f aca="false">SUM(J3:J53)/500</f>
         <v>40.75524</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
-      <c r="B61" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="B62" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" s="5" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="63">
+      <c r="B63" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="64">
+      <c r="B64" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" s="5" t="n">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="63">
-      <c r="B63" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E63" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="65">
+      <c r="B65" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" s="0" t="n">
         <v>69.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
-      <c r="B71" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
-      <c r="B72" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E72" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F72" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
+      <c r="B73" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
+      <c r="B74" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="0" t="n">
         <v>4.04</v>
       </c>
-      <c r="G72" s="0" t="n">
-        <f aca="false">F72*E72</f>
+      <c r="G74" s="0" t="n">
+        <f aca="false">F74*E74</f>
         <v>4.04</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
-      <c r="B73" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="E73" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F73" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
+      <c r="B75" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="G73" s="0" t="n">
-        <f aca="false">F73*E73</f>
+      <c r="G75" s="0" t="n">
+        <f aca="false">F75*E75</f>
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
-      <c r="B74" s="5" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="76">
+      <c r="B76" s="5" t="n">
         <v>889740626</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F74" s="0" t="n">
+      <c r="C76" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G74" s="18" t="n">
-        <f aca="false">F74*E74</f>
+      <c r="G76" s="18" t="n">
+        <f aca="false">F76*E76</f>
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
-      <c r="B75" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="G75" s="1" t="n">
-        <f aca="false">SUM(G72:G74)</f>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="77">
+      <c r="B77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="G77" s="1" t="n">
+        <f aca="false">SUM(G74:G76)</f>
         <v>33.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
No more airwires, now starts the DRC work
</commit_message>
<xml_diff>
--- a/PCB_rev_A2/Replicape_BOM_rev_A2.xlsx
+++ b/PCB_rev_A2/Replicape_BOM_rev_A2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
   <si>
     <t>Implemented</t>
   </si>
@@ -414,24 +414,6 @@
   </si>
   <si>
     <t>S1</t>
-  </si>
-  <si>
-    <t>RUEF900-ND</t>
-  </si>
-  <si>
-    <t>POLYSWITCH RUE SERIES 9.00A</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>RGEF500-ND</t>
-  </si>
-  <si>
-    <t>POLYSWITCH RGE SERIES 5.0A HOLD</t>
-  </si>
-  <si>
-    <t>F1, F3</t>
   </si>
   <si>
     <t>MBRA340T3GOSCT-ND</t>
@@ -703,10 +685,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A54" activeCellId="0" pane="topLeft" sqref="A54"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C54" activeCellId="0" pane="topLeft" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -2267,25 +2249,25 @@
         <v>135</v>
       </c>
       <c r="E54" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F54" s="7" t="n">
-        <v>0.83</v>
+        <v>6</v>
+      </c>
+      <c r="F54" s="6" t="n">
+        <v>0.53</v>
       </c>
       <c r="G54" s="7" t="n">
         <f aca="false">E54*F54</f>
-        <v>0.83</v>
+        <v>3.18</v>
       </c>
       <c r="H54" s="7" t="n">
         <f aca="false">E54*500</f>
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="I54" s="6" t="n">
-        <v>0.5421</v>
+        <v>0.24812</v>
       </c>
       <c r="J54" s="7" t="n">
         <f aca="false">H54*I54</f>
-        <v>271.05</v>
+        <v>744.36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55" s="5">
@@ -2302,25 +2284,25 @@
         <v>138</v>
       </c>
       <c r="E55" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F55" s="7" t="n">
-        <v>0.56</v>
+        <v>1</v>
+      </c>
+      <c r="F55" s="6" t="n">
+        <v>0.45</v>
       </c>
       <c r="G55" s="7" t="n">
         <f aca="false">E55*F55</f>
-        <v>1.12</v>
+        <v>0.45</v>
       </c>
       <c r="H55" s="7" t="n">
         <f aca="false">E55*500</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I55" s="6" t="n">
-        <v>0.36076</v>
+        <v>0.26</v>
       </c>
       <c r="J55" s="7" t="n">
         <f aca="false">H55*I55</f>
-        <v>360.76</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56" s="5">
@@ -2337,25 +2319,25 @@
         <v>141</v>
       </c>
       <c r="E56" s="7" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>0.53</v>
+        <v>0.57</v>
       </c>
       <c r="G56" s="7" t="n">
         <f aca="false">E56*F56</f>
-        <v>3.18</v>
+        <v>0.57</v>
       </c>
       <c r="H56" s="7" t="n">
         <f aca="false">E56*500</f>
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="I56" s="6" t="n">
-        <v>0.24812</v>
+        <v>0.37126</v>
       </c>
       <c r="J56" s="7" t="n">
         <f aca="false">H56*I56</f>
-        <v>744.36</v>
+        <v>185.63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57" s="5">
@@ -2375,22 +2357,19 @@
         <v>1</v>
       </c>
       <c r="F57" s="6" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="G57" s="7" t="n">
         <f aca="false">E57*F57</f>
-        <v>0.45</v>
-      </c>
-      <c r="H57" s="7" t="n">
-        <f aca="false">E57*500</f>
-        <v>500</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="H57" s="7"/>
       <c r="I57" s="6" t="n">
-        <v>0.26</v>
+        <v>0.204</v>
       </c>
       <c r="J57" s="7" t="n">
         <f aca="false">H57*I57</f>
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58" s="5">
@@ -2410,229 +2389,164 @@
         <v>1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>0.57</v>
+        <v>0.47</v>
       </c>
       <c r="G58" s="7" t="n">
         <f aca="false">E58*F58</f>
-        <v>0.57</v>
-      </c>
-      <c r="H58" s="7" t="n">
-        <f aca="false">E58*500</f>
-        <v>500</v>
-      </c>
+        <v>0.47</v>
+      </c>
+      <c r="H58" s="7"/>
       <c r="I58" s="6" t="n">
-        <v>0.37126</v>
+        <v>0.34</v>
       </c>
       <c r="J58" s="7" t="n">
         <f aca="false">H58*I58</f>
-        <v>185.63</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59" s="5">
-      <c r="A59" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B59" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="B59" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E59" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F59" s="6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G59" s="7" t="n">
-        <f aca="false">E59*F59</f>
-        <v>0.4</v>
-      </c>
-      <c r="H59" s="7"/>
-      <c r="I59" s="6" t="n">
-        <v>0.204</v>
-      </c>
-      <c r="J59" s="7" t="n">
-        <f aca="false">H59*I59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60" s="5">
-      <c r="A60" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E60" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" s="6" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="G60" s="7" t="n">
-        <f aca="false">E60*F60</f>
-        <v>0.47</v>
-      </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="6" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="J60" s="7" t="n">
-        <f aca="false">H60*I60</f>
-        <v>0</v>
-      </c>
-    </row>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="n">
+        <f aca="false">SUM(G3:G58)</f>
+        <v>89.983</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1" t="n">
+        <f aca="false">SUM(J3:J53)/500</f>
+        <v>40.75524</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="B61" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="B62" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="5" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="63">
+      <c r="B63" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1" t="n">
-        <f aca="false">SUM(G3:G60)</f>
-        <v>91.933</v>
-      </c>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1" t="n">
-        <f aca="false">SUM(J3:J53)/500</f>
-        <v>40.75524</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="63">
-      <c r="B63" s="1" t="s">
+      <c r="D63" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>69.95</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
+      <c r="B71" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="B64" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
+      <c r="B72" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D72" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="E64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" s="5" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="65">
-      <c r="B65" s="14" t="s">
+      <c r="E72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <f aca="false">F72*E72</f>
+        <v>4.04</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
+      <c r="B73" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C73" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>69.95</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
-      <c r="B73" s="1" t="s">
+      <c r="D73" s="0" t="s">
         <v>161</v>
       </c>
+      <c r="E73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <f aca="false">F73*E73</f>
+        <v>9</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="5" t="n">
+        <v>889740626</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="D74" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="E74" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G74" s="18" t="n">
+        <f aca="false">F74*E74</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
+      <c r="B75" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>4.04</v>
-      </c>
-      <c r="G74" s="0" t="n">
-        <f aca="false">F74*E74</f>
-        <v>4.04</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
-      <c r="B75" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G75" s="0" t="n">
-        <f aca="false">F75*E75</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="76">
-      <c r="B76" s="5" t="n">
-        <v>889740626</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="E76" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G76" s="18" t="n">
-        <f aca="false">F76*E76</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="77">
-      <c r="B77" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="G77" s="1" t="n">
-        <f aca="false">SUM(G74:G76)</f>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="G75" s="1" t="n">
+        <f aca="false">SUM(G72:G74)</f>
         <v>33.04</v>
       </c>
     </row>

</xml_diff>